<commit_message>
Uptade new data functional and columns name in dicts
</commit_message>
<xml_diff>
--- a/codes/periods.xlsx
+++ b/codes/periods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\d\Projects\!Projects\PG_portal\script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyzhur\Git\GP\pg_dt_portal\codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98955C51-6060-48AD-B6D0-65F62F9A3BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246D7ED7-D1BA-49E5-BA4C-9789C73A06CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="period_lbl" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
   <si>
     <t>2MATs: Mar 2023</t>
   </si>
@@ -329,12 +329,6 @@
     <t>Month: Mar 2024</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
     <t>3MMT/ 12we</t>
   </si>
   <si>
@@ -660,19 +654,44 @@
   </si>
   <si>
     <t>label_num</t>
+  </si>
+  <si>
+    <t>period_lbl</t>
+  </si>
+  <si>
+    <t>time_period_type</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>period_code</t>
+  </si>
+  <si>
+    <t>time_period_code</t>
+  </si>
+  <si>
+    <t>year_code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -695,11 +714,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -979,21 +1001,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
+        <v>212</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="C1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1004,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1015,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1026,7 +1046,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1037,7 +1057,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1048,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1059,7 +1079,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1070,7 +1090,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1081,7 +1101,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1092,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1103,7 +1123,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1114,7 +1134,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1125,7 +1145,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1136,7 +1156,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1147,7 +1167,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1158,7 +1178,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1169,7 +1189,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1180,7 +1200,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1191,7 +1211,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1202,7 +1222,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1213,7 +1233,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1224,7 +1244,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1235,7 +1255,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1246,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1257,7 +1277,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1268,7 +1288,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1279,7 +1299,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1290,7 +1310,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1301,7 +1321,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1312,7 +1332,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1323,7 +1343,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1334,7 +1354,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1345,7 +1365,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1356,7 +1376,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1367,7 +1387,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1378,7 +1398,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1389,7 +1409,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1400,7 +1420,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1411,7 +1431,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1422,7 +1442,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1433,7 +1453,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1444,7 +1464,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1455,7 +1475,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1466,7 +1486,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1477,7 +1497,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1488,7 +1508,7 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1499,7 +1519,7 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1510,7 +1530,7 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1521,7 +1541,7 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1532,7 +1552,7 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1543,7 +1563,7 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1554,7 +1574,7 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1565,7 +1585,7 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1576,7 +1596,7 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1587,7 +1607,7 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1598,7 +1618,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1609,7 +1629,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1620,7 +1640,7 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1631,7 +1651,7 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1642,7 +1662,7 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1653,7 +1673,7 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1664,7 +1684,7 @@
         <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1675,7 +1695,7 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1686,7 +1706,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1697,7 +1717,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1708,7 +1728,7 @@
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1719,7 +1739,7 @@
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1730,7 +1750,7 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1741,7 +1761,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1752,7 +1772,7 @@
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1763,7 +1783,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1774,7 +1794,7 @@
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1785,7 +1805,7 @@
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1796,7 +1816,7 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1807,7 +1827,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1818,7 +1838,7 @@
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1829,7 +1849,7 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1840,7 +1860,7 @@
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1851,7 +1871,7 @@
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1862,7 +1882,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1873,7 +1893,7 @@
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1884,7 +1904,7 @@
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1895,7 +1915,7 @@
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1906,7 +1926,7 @@
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1917,7 +1937,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1928,7 +1948,7 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1939,7 +1959,7 @@
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1950,7 +1970,7 @@
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1961,7 +1981,7 @@
         <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1972,7 +1992,7 @@
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -1983,7 +2003,7 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -1994,7 +2014,7 @@
         <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -2005,7 +2025,7 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -2016,7 +2036,7 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -2027,7 +2047,7 @@
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -2038,7 +2058,7 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -2049,7 +2069,7 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2060,7 +2080,7 @@
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -2071,7 +2091,7 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -2082,7 +2102,7 @@
         <v>98</v>
       </c>
       <c r="C100" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -2093,11 +2113,12 @@
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2106,17 +2127,17 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
+        <v>213</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2124,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2132,7 +2153,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2140,7 +2161,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2148,7 +2169,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2160,18 +2181,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB13A4A-EC37-405A-8A8F-7ED848F7999D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>214</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2179,7 +2200,7 @@
         <v>2021</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2187,7 +2208,7 @@
         <v>2022</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2195,7 +2216,7 @@
         <v>2023</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2203,7 +2224,7 @@
         <v>2024</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add mask for columns, match columns name, rename columns in sav script
</commit_message>
<xml_diff>
--- a/codes/periods.xlsx
+++ b/codes/periods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyzhur\Git\GP\pg_dt_portal\codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyzhur\Git\GP\PG_Clone\pg-dt-portal-for-nz\codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246D7ED7-D1BA-49E5-BA4C-9789C73A06CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37885952-2F25-4F71-9CAD-84DD24B5A5A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="period_lbl" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <si>
     <t>2MATs: Mar 2023</t>
   </si>
@@ -335,9 +335,6 @@
     <t>MAT/ 52 we</t>
   </si>
   <si>
-    <t>2MAT/ 104 we</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -672,6 +669,33 @@
   </si>
   <si>
     <t>year_code</t>
+  </si>
+  <si>
+    <t>2MATs: Jun 2024</t>
+  </si>
+  <si>
+    <t>Month: 2024 (06) Jun</t>
+  </si>
+  <si>
+    <t>2MATs: 2024 (06) Jun</t>
+  </si>
+  <si>
+    <t>MAT: Jun 2024</t>
+  </si>
+  <si>
+    <t>MAT: 2024 (06) Jun</t>
+  </si>
+  <si>
+    <t>Month: Jun 2024</t>
+  </si>
+  <si>
+    <t>3MMT: Jun 2024</t>
+  </si>
+  <si>
+    <t>3MMT: 2024 (06) Jun</t>
+  </si>
+  <si>
+    <t>2MATs/ 104 we</t>
   </si>
 </sst>
 </file>
@@ -999,21 +1023,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1024,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1035,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1046,7 +1075,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1057,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1068,7 +1097,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1079,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1090,7 +1119,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1101,7 +1130,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1112,7 +1141,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1123,7 +1152,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1134,7 +1163,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1145,7 +1174,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1156,7 +1185,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1167,7 +1196,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1178,7 +1207,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1189,7 +1218,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1200,7 +1229,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1211,7 +1240,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1222,7 +1251,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1233,7 +1262,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1244,7 +1273,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1255,7 +1284,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1266,7 +1295,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1277,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1288,7 +1317,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1299,7 +1328,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -1310,7 +1339,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -1321,7 +1350,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1332,7 +1361,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -1343,7 +1372,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -1354,7 +1383,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1365,7 +1394,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1376,7 +1405,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1387,7 +1416,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1398,7 +1427,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1409,7 +1438,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1420,7 +1449,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1431,7 +1460,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1442,7 +1471,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1453,7 +1482,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1464,7 +1493,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1475,7 +1504,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1486,7 +1515,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1497,7 +1526,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1508,7 +1537,7 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1519,7 +1548,7 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1530,7 +1559,7 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1541,7 +1570,7 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1552,7 +1581,7 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1563,7 +1592,7 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1574,7 +1603,7 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1585,7 +1614,7 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1596,7 +1625,7 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1607,7 +1636,7 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1618,7 +1647,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1629,7 +1658,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1640,7 +1669,7 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1651,7 +1680,7 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1662,7 +1691,7 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1673,7 +1702,7 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1684,7 +1713,7 @@
         <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1695,7 +1724,7 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1706,7 +1735,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1717,7 +1746,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1728,7 +1757,7 @@
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1739,7 +1768,7 @@
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1750,7 +1779,7 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1761,7 +1790,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1772,7 +1801,7 @@
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1783,7 +1812,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1794,7 +1823,7 @@
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1805,7 +1834,7 @@
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1816,7 +1845,7 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1827,7 +1856,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1838,7 +1867,7 @@
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1849,7 +1878,7 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1860,7 +1889,7 @@
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1871,7 +1900,7 @@
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1882,7 +1911,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1893,7 +1922,7 @@
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1904,7 +1933,7 @@
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1915,7 +1944,7 @@
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1926,7 +1955,7 @@
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1937,7 +1966,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1948,7 +1977,7 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1959,7 +1988,7 @@
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1970,7 +1999,7 @@
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1981,7 +2010,7 @@
         <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1992,7 +2021,7 @@
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -2003,7 +2032,7 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -2014,7 +2043,7 @@
         <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -2025,7 +2054,7 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -2036,7 +2065,7 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -2047,7 +2076,7 @@
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -2058,7 +2087,7 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -2069,7 +2098,7 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2080,7 +2109,7 @@
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -2091,7 +2120,7 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -2102,7 +2131,7 @@
         <v>98</v>
       </c>
       <c r="C100" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -2113,7 +2142,51 @@
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>207</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>214</v>
+      </c>
+      <c r="C102" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>217</v>
+      </c>
+      <c r="C103" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>219</v>
+      </c>
+      <c r="C104" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>220</v>
+      </c>
+      <c r="C105" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2126,18 +2199,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F682F912-283F-40E7-8E59-3B2EEFCFE15E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2161,7 +2234,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2169,7 +2242,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2181,7 +2254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB13A4A-EC37-405A-8A8F-7ED848F7999D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2189,10 +2262,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2200,7 +2273,7 @@
         <v>2021</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2208,7 +2281,7 @@
         <v>2022</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2216,7 +2289,7 @@
         <v>2023</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2224,7 +2297,7 @@
         <v>2024</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new perionds in dict
</commit_message>
<xml_diff>
--- a/codes/periods.xlsx
+++ b/codes/periods.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\d\Projects\!Projects\PG_portal\script\codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nyzhur\Git\pg-dt-portal-for-nz\codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD6FFE6-FA3B-4BEB-B93A-937CAC8FE4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE5F0C0-A511-4B6F-984E-30BF4B454182}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="period_lbl" sheetId="1" r:id="rId1"/>
     <sheet name="time_period_type" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="255">
   <si>
     <t>2MATs: Mar 2023</t>
   </si>
@@ -732,6 +732,66 @@
   </si>
   <si>
     <t>Month</t>
+  </si>
+  <si>
+    <t>MAT: Sep 2024</t>
+  </si>
+  <si>
+    <t>2MATs: Sep 2024</t>
+  </si>
+  <si>
+    <t>3MMT: Sep 2024</t>
+  </si>
+  <si>
+    <t>Month: Jul 2024</t>
+  </si>
+  <si>
+    <t>Month: Sep 2024</t>
+  </si>
+  <si>
+    <t>MAT: Jul 2024</t>
+  </si>
+  <si>
+    <t>MAT: Aug 2024</t>
+  </si>
+  <si>
+    <t>3MMT: Aug 2024</t>
+  </si>
+  <si>
+    <t>Month: Aug 2024</t>
+  </si>
+  <si>
+    <t>3MMT: Jul 2024</t>
+  </si>
+  <si>
+    <t>2MATs: 2024 (09) Sep</t>
+  </si>
+  <si>
+    <t>3MMT: 2024 (07) Jul</t>
+  </si>
+  <si>
+    <t>3MMT: 2024 (08) Aug</t>
+  </si>
+  <si>
+    <t>3MMT: 2024 (09) Sep</t>
+  </si>
+  <si>
+    <t>MAT: 2024 (08) Aug</t>
+  </si>
+  <si>
+    <t>MAT: 2024 (07) Jul</t>
+  </si>
+  <si>
+    <t>MAT: 2024 (09) Sep</t>
+  </si>
+  <si>
+    <t>Month: 2024 (08) Aug</t>
+  </si>
+  <si>
+    <t>Month: 2024 (07) Jul</t>
+  </si>
+  <si>
+    <t>Month: 2024 (09) Sep</t>
   </si>
 </sst>
 </file>
@@ -747,7 +807,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -757,6 +817,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,12 +839,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1056,15 +1124,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="30.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -2288,7 +2358,121 @@
         <v>214</v>
       </c>
     </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A113:D121">
+    <sortCondition ref="A113:A121"/>
+    <sortCondition ref="D113:D121"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2298,7 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F682F912-283F-40E7-8E59-3B2EEFCFE15E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update to new upload backdata in nwe format
</commit_message>
<xml_diff>
--- a/codes/periods.xlsx
+++ b/codes/periods.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -591,7 +591,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -614,7 +614,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -660,7 +660,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -683,7 +683,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -706,7 +706,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -729,7 +729,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -752,7 +752,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -775,7 +775,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -798,7 +798,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -821,7 +821,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -844,7 +844,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -890,7 +890,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -913,7 +913,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -936,7 +936,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -959,7 +959,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -982,7 +982,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -1879,7 +1879,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2017,7 +2017,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -2178,7 +2178,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -2224,7 +2224,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2477,7 +2477,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -2523,7 +2523,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -2684,7 +2684,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E97" t="n">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -2776,7 +2776,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -2983,7 +2983,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -3052,7 +3052,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -3075,7 +3075,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -3144,7 +3144,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -3328,7 +3328,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -3351,7 +3351,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -3397,7 +3397,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -3420,7 +3420,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E128" t="n">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -3512,7 +3512,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E131" t="n">
@@ -3535,7 +3535,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -3627,7 +3627,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -3650,7 +3650,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E137" t="n">
@@ -3673,7 +3673,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E138" t="n">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E140" t="n">
@@ -3742,7 +3742,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E141" t="n">
@@ -3765,7 +3765,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E142" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E143" t="n">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E144" t="n">
@@ -3834,7 +3834,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>2025-01-14</t>
+          <t>2025-01-15</t>
         </is>
       </c>
       <c r="E145" t="n">

</xml_diff>